<commit_message>
Messed around with create grid algo
</commit_message>
<xml_diff>
--- a/Grids/GetToGrid_Week1.xlsx
+++ b/Grids/GetToGrid_Week1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="91">
   <si>
     <t>Activity</t>
   </si>
@@ -187,19 +187,106 @@
     <t>11:00-11:45</t>
   </si>
   <si>
-    <t>Nono</t>
-  </si>
-  <si>
-    <t>NONE FOUND</t>
+    <t>Smiles</t>
+  </si>
+  <si>
+    <t>Queen-E</t>
+  </si>
+  <si>
+    <t>Sea</t>
+  </si>
+  <si>
+    <t>Nodder</t>
+  </si>
+  <si>
+    <t>Ups</t>
+  </si>
+  <si>
+    <t>G-Poppy</t>
+  </si>
+  <si>
+    <t>Surf Co</t>
+  </si>
+  <si>
+    <t>Indi</t>
+  </si>
+  <si>
+    <t>Tross</t>
+  </si>
+  <si>
+    <t>Bow Wow</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Bops</t>
+  </si>
+  <si>
+    <t>Goobie</t>
+  </si>
+  <si>
+    <t>Blister</t>
+  </si>
+  <si>
+    <t>Opps</t>
+  </si>
+  <si>
+    <t>Hoops</t>
+  </si>
+  <si>
+    <t>Unicorn</t>
+  </si>
+  <si>
+    <t>Jaws</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Laddy</t>
+  </si>
+  <si>
+    <t>Packs</t>
+  </si>
+  <si>
+    <t>Burning Bush</t>
+  </si>
+  <si>
+    <t>GoGo</t>
+  </si>
+  <si>
+    <t>Nom Nom</t>
+  </si>
+  <si>
+    <t>Dad</t>
+  </si>
+  <si>
+    <t>Bonez</t>
+  </si>
+  <si>
+    <t>Stastro</t>
+  </si>
+  <si>
+    <t>Captain</t>
   </si>
   <si>
     <t>Claps</t>
   </si>
   <si>
-    <t>Hoops</t>
-  </si>
-  <si>
-    <t>Padge</t>
+    <t>T-Whisk</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Gaggles</t>
+  </si>
+  <si>
+    <t>Geni</t>
+  </si>
+  <si>
+    <t>Acro</t>
   </si>
 </sst>
 </file>
@@ -600,19 +687,19 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -626,19 +713,19 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -652,10 +739,10 @@
         <v>35</v>
       </c>
       <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
         <v>61</v>
-      </c>
-      <c r="I4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -669,10 +756,10 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" t="s">
         <v>60</v>
-      </c>
-      <c r="I5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -686,19 +773,19 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="G6" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -712,19 +799,19 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="G7" t="s">
         <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="I7" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -749,7 +836,7 @@
         <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -763,7 +850,7 @@
         <v>38</v>
       </c>
       <c r="I10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -777,7 +864,7 @@
         <v>39</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -791,7 +878,7 @@
         <v>39</v>
       </c>
       <c r="I12" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -805,7 +892,7 @@
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -819,10 +906,10 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -836,10 +923,10 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F15" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -853,10 +940,10 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -870,16 +957,16 @@
         <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="I17" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -896,13 +983,13 @@
         <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="I18" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -927,7 +1014,7 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -941,7 +1028,7 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -955,7 +1042,7 @@
         <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -969,7 +1056,7 @@
         <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -983,19 +1070,19 @@
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="H24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I24" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1009,19 +1096,19 @@
         <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I25" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1038,19 +1125,19 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="G26" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="H26" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I26" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1067,19 +1154,19 @@
         <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="G27" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="H27" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="I27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1093,22 +1180,22 @@
         <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="G28" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="H28" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="I28" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1122,22 +1209,22 @@
         <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="G29" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="H29" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="I29" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1151,19 +1238,19 @@
         <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F30" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="G30" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="H30" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="I30" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1177,10 +1264,10 @@
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H31" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1194,10 +1281,10 @@
         <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="H32" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1211,19 +1298,19 @@
         <v>49</v>
       </c>
       <c r="E33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" t="s">
         <v>59</v>
       </c>
-      <c r="F33" t="s">
-        <v>59</v>
-      </c>
-      <c r="G33" t="s">
-        <v>59</v>
-      </c>
-      <c r="H33" t="s">
-        <v>61</v>
-      </c>
       <c r="I33" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1237,19 +1324,19 @@
         <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F34" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G34" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="H34" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I34" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1263,19 +1350,19 @@
         <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G35" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="H35" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="I35" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1289,19 +1376,19 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F36" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="G36" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="H36" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="I36" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1315,22 +1402,22 @@
         <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="F37" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="G37" t="s">
         <v>59</v>
       </c>
       <c r="H37" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="I37" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1344,13 +1431,13 @@
         <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="G38" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="I38" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1364,13 +1451,13 @@
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G39" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="I39" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1384,13 +1471,13 @@
         <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G40" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="I40" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1404,19 +1491,19 @@
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F41" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G41" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="H41" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="I41" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1430,19 +1517,19 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F42" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G42" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I42" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1456,19 +1543,19 @@
         <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="F43" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="G43" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="H43" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="I43" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1482,19 +1569,19 @@
         <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="F44" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="G44" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="H44" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="I44" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1508,19 +1595,19 @@
         <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F45" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="G45" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="H45" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="I45" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1534,13 +1621,13 @@
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="G46" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1554,13 +1641,13 @@
         <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I47" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1574,10 +1661,10 @@
         <v>52</v>
       </c>
       <c r="F48" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="H48" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1591,16 +1678,16 @@
         <v>47</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="F49" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="H49" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="I49" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1614,10 +1701,10 @@
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="H50" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1631,10 +1718,10 @@
         <v>48</v>
       </c>
       <c r="F51" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="H51" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1648,10 +1735,10 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="G52" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1676,10 +1763,10 @@
         <v>54</v>
       </c>
       <c r="F54" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="H54" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1693,10 +1780,10 @@
         <v>54</v>
       </c>
       <c r="F55" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="H55" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1710,10 +1797,10 @@
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E56" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -1727,10 +1814,10 @@
         <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E57" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -1744,10 +1831,10 @@
         <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E58" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -1761,13 +1848,13 @@
         <v>55</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="F59" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H59" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -1781,22 +1868,22 @@
         <v>55</v>
       </c>
       <c r="D60" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E60" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="F60" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="G60" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H60" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="I60" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -1810,22 +1897,22 @@
         <v>56</v>
       </c>
       <c r="D61" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E61" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="F61" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G61" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="H61" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I61" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -1839,22 +1926,22 @@
         <v>56</v>
       </c>
       <c r="D62" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E62" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="F62" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="G62" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="H62" t="s">
         <v>60</v>
       </c>
       <c r="I62" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added to create grid algo and renamed and moved permanent data
</commit_message>
<xml_diff>
--- a/Grids/GetToGrid_Week1.xlsx
+++ b/Grids/GetToGrid_Week1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="151">
   <si>
     <t>Activity</t>
   </si>
@@ -187,106 +187,286 @@
     <t>11:00-11:45</t>
   </si>
   <si>
-    <t>Smiles</t>
-  </si>
-  <si>
-    <t>Queen-E</t>
-  </si>
-  <si>
-    <t>Sea</t>
-  </si>
-  <si>
-    <t>Nodder</t>
-  </si>
-  <si>
-    <t>Ups</t>
-  </si>
-  <si>
-    <t>G-Poppy</t>
-  </si>
-  <si>
-    <t>Surf Co</t>
-  </si>
-  <si>
-    <t>Indi</t>
-  </si>
-  <si>
-    <t>Tross</t>
-  </si>
-  <si>
-    <t>Bow Wow</t>
-  </si>
-  <si>
-    <t>Zombie</t>
-  </si>
-  <si>
-    <t>Bops</t>
-  </si>
-  <si>
-    <t>Goobie</t>
-  </si>
-  <si>
-    <t>Blister</t>
-  </si>
-  <si>
-    <t>Opps</t>
-  </si>
-  <si>
-    <t>Hoops</t>
-  </si>
-  <si>
-    <t>Unicorn</t>
-  </si>
-  <si>
-    <t>Jaws</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Laddy</t>
-  </si>
-  <si>
-    <t>Packs</t>
-  </si>
-  <si>
-    <t>Burning Bush</t>
-  </si>
-  <si>
-    <t>GoGo</t>
-  </si>
-  <si>
-    <t>Nom Nom</t>
-  </si>
-  <si>
-    <t>Dad</t>
-  </si>
-  <si>
-    <t>Bonez</t>
-  </si>
-  <si>
-    <t>Stastro</t>
-  </si>
-  <si>
-    <t>Captain</t>
-  </si>
-  <si>
-    <t>Claps</t>
-  </si>
-  <si>
-    <t>T-Whisk</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Gaggles</t>
-  </si>
-  <si>
-    <t>Geni</t>
-  </si>
-  <si>
-    <t>Acro</t>
+    <t>Nodder Male['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Unicorn Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Opps Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Bow Wow Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Zombie Male['']</t>
+  </si>
+  <si>
+    <t>Nono Male['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Hoops Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>T-Whisk Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Nom Nom Female['']</t>
+  </si>
+  <si>
+    <t>Acro Male['Leadership', 'Male']</t>
+  </si>
+  <si>
+    <t>Zombie Male['Male']</t>
+  </si>
+  <si>
+    <t>Nono Male['']</t>
+  </si>
+  <si>
+    <t>Goobie Female['']</t>
+  </si>
+  <si>
+    <t>Indi Male['']</t>
+  </si>
+  <si>
+    <t>Jaws Male['']</t>
+  </si>
+  <si>
+    <t>Dad Female['Female', 'Leadership']</t>
+  </si>
+  <si>
+    <t>Smiles Female['Female']</t>
+  </si>
+  <si>
+    <t>Laddy Male['Lifegaurd', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Burning Bush Male['Lifegaurd', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Bonez Female['Lifegaurd', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Captain Male['Non-program']</t>
+  </si>
+  <si>
+    <t>Bow Wow Female['Non-program']</t>
+  </si>
+  <si>
+    <t>Tross Male['Lifegaurd', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Pizza Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Ups Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Nom Nom Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Smiles Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Goobie Female['Female']</t>
+  </si>
+  <si>
+    <t>Opps Female['Female']</t>
+  </si>
+  <si>
+    <t>Hoops Female['Female']</t>
+  </si>
+  <si>
+    <t>T-Whisk Female['Female']</t>
+  </si>
+  <si>
+    <t>Captain Male['']</t>
+  </si>
+  <si>
+    <t>Stastro Male['']</t>
+  </si>
+  <si>
+    <t>Chicken Female['']</t>
+  </si>
+  <si>
+    <t>G-Poppy Female['Ropes']</t>
+  </si>
+  <si>
+    <t>Laddy Male['Ropes']</t>
+  </si>
+  <si>
+    <t>Burning Bush Male['Ropes']</t>
+  </si>
+  <si>
+    <t>Bow Wow Female['Ropes']</t>
+  </si>
+  <si>
+    <t>Nodder Male['Ropes']</t>
+  </si>
+  <si>
+    <t>Blister Male['Ropes']</t>
+  </si>
+  <si>
+    <t>GoGo Female['Female']</t>
+  </si>
+  <si>
+    <t>Unicorn Female['Female']</t>
+  </si>
+  <si>
+    <t>Indi Male['Male']</t>
+  </si>
+  <si>
+    <t>GoGo Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Surf Co Male['']</t>
+  </si>
+  <si>
+    <t>Opps Female['']</t>
+  </si>
+  <si>
+    <t>Stastro Male['Male']</t>
+  </si>
+  <si>
+    <t>Sea Female['']</t>
+  </si>
+  <si>
+    <t>Chicken Female['Lifegaurd', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Sea Female['Non-program']</t>
+  </si>
+  <si>
+    <t>Indi Male['Non-program']</t>
+  </si>
+  <si>
+    <t>Laddy Male['Male', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Burning Bush Male['Male', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Sea Female['Lifegaurd', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Chicken Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Indi Male['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Captain Male['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Bonez Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>G-Poppy Female['']</t>
+  </si>
+  <si>
+    <t>T-Whisk Female['']</t>
+  </si>
+  <si>
+    <t>Bow Wow Female['Female']</t>
+  </si>
+  <si>
+    <t>Stastro Male['Ropes']</t>
+  </si>
+  <si>
+    <t>Pizza Female['Ropes']</t>
+  </si>
+  <si>
+    <t>NONE FOUND</t>
+  </si>
+  <si>
+    <t>Tross Male['Male']</t>
+  </si>
+  <si>
+    <t>Laddy Male['Male']</t>
+  </si>
+  <si>
+    <t>Burning Bush Male['Male']</t>
+  </si>
+  <si>
+    <t>Surf Co Male['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Blister Male['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Tross Male['']</t>
+  </si>
+  <si>
+    <t>Hoops Female['']</t>
+  </si>
+  <si>
+    <t>GoGo Female['']</t>
+  </si>
+  <si>
+    <t>Indi Male['Lifegaurd', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Bow Wow Female['Lifegaurd', 'Non-program']</t>
+  </si>
+  <si>
+    <t>Jaws Male['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Chicken Female['Female']</t>
+  </si>
+  <si>
+    <t>Bonez Female['Female']</t>
+  </si>
+  <si>
+    <t>Pizza Female['Female']</t>
+  </si>
+  <si>
+    <t>Blister Male['']</t>
+  </si>
+  <si>
+    <t>Burning Bush Male['']</t>
+  </si>
+  <si>
+    <t>Sea Female['Female']</t>
+  </si>
+  <si>
+    <t>Nono Male['Male']</t>
+  </si>
+  <si>
+    <t>Laddy Male['Non-program']</t>
+  </si>
+  <si>
+    <t>Burning Bush Male['Non-program']</t>
+  </si>
+  <si>
+    <t>Zombie Male['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Ups Female['Female']</t>
+  </si>
+  <si>
+    <t>Surf Co Male['Male']</t>
+  </si>
+  <si>
+    <t>Pizza Female['']</t>
+  </si>
+  <si>
+    <t>Bow Wow Female['']</t>
+  </si>
+  <si>
+    <t>Bow Wow Female['Ropes', 'Non-program']</t>
+  </si>
+  <si>
+    <t>T-Whisk Female['Ropes', 'Non-program']</t>
+  </si>
+  <si>
+    <t>G-Poppy Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Goobie Female['Lifegaurd']</t>
+  </si>
+  <si>
+    <t>Laddy Male['']</t>
   </si>
 </sst>
 </file>
@@ -687,19 +867,19 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
       <c r="H2" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -713,19 +893,19 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" t="s">
         <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" t="s">
-        <v>86</v>
-      </c>
-      <c r="H3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -739,10 +919,10 @@
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -756,10 +936,10 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I5" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -773,19 +953,19 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I6" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -799,19 +979,19 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="H7" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -836,7 +1016,7 @@
         <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -850,7 +1030,7 @@
         <v>38</v>
       </c>
       <c r="I10" t="s">
-        <v>60</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -864,7 +1044,7 @@
         <v>39</v>
       </c>
       <c r="I11" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -878,7 +1058,7 @@
         <v>39</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -892,7 +1072,7 @@
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -906,10 +1086,10 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -923,10 +1103,10 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -940,10 +1120,10 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -957,16 +1137,16 @@
         <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F17" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="H17" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -980,16 +1160,16 @@
         <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1014,7 +1194,7 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1028,7 +1208,7 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1042,7 +1222,7 @@
         <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1056,7 +1236,7 @@
         <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1070,19 +1250,19 @@
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" t="s">
+        <v>129</v>
+      </c>
+      <c r="H24" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" t="s">
         <v>74</v>
-      </c>
-      <c r="G24" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" t="s">
-        <v>59</v>
-      </c>
-      <c r="I24" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1096,19 +1276,19 @@
         <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="H25" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
       <c r="I25" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1125,19 +1305,19 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
       <c r="G26" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="H26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I26" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1154,16 +1334,16 @@
         <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="G27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H27" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="I27" t="s">
         <v>58</v>
@@ -1183,19 +1363,19 @@
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F28" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="H28" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="I28" t="s">
-        <v>81</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1212,19 +1392,19 @@
         <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="F29" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="G29" t="s">
-        <v>88</v>
+        <v>131</v>
       </c>
       <c r="H29" t="s">
-        <v>62</v>
+        <v>141</v>
       </c>
       <c r="I29" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1238,19 +1418,19 @@
         <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="F30" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="G30" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="H30" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="I30" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1264,10 +1444,10 @@
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="H31" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1281,10 +1461,10 @@
         <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="H32" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1298,19 +1478,19 @@
         <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F33" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G33" t="s">
-        <v>68</v>
+        <v>132</v>
       </c>
       <c r="H33" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="I33" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1324,19 +1504,19 @@
         <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="F34" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="G34" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="H34" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="I34" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1350,19 +1530,19 @@
         <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>58</v>
+        <v>86</v>
       </c>
       <c r="F35" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="G35" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="H35" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="I35" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1376,19 +1556,19 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="F36" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="G36" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="H36" t="s">
-        <v>67</v>
+        <v>134</v>
       </c>
       <c r="I36" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1405,19 +1585,19 @@
         <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F37" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="G37" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="H37" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="I37" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1431,13 +1611,13 @@
         <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="G38" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="I38" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1451,13 +1631,13 @@
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="G39" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="I39" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1471,13 +1651,13 @@
         <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="G40" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="I40" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1491,19 +1671,19 @@
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="F41" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="G41" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="H41" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="I41" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1517,19 +1697,19 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="F42" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="G42" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="H42" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="I42" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1543,19 +1723,19 @@
         <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="F43" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="H43" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="I43" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1569,19 +1749,19 @@
         <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="F44" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="G44" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="H44" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="I44" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1595,19 +1775,19 @@
         <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="F45" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="G45" t="s">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="H45" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="I45" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1621,13 +1801,13 @@
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="G46" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="I46" t="s">
-        <v>61</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1641,13 +1821,13 @@
         <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="G47" t="s">
-        <v>57</v>
+        <v>137</v>
       </c>
       <c r="I47" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1661,10 +1841,10 @@
         <v>52</v>
       </c>
       <c r="F48" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="H48" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1678,16 +1858,16 @@
         <v>47</v>
       </c>
       <c r="E49" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="F49" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="H49" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
       <c r="I49" t="s">
-        <v>75</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1701,10 +1881,10 @@
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="H50" t="s">
-        <v>67</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1718,10 +1898,10 @@
         <v>48</v>
       </c>
       <c r="F51" t="s">
-        <v>76</v>
+        <v>123</v>
       </c>
       <c r="H51" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1735,10 +1915,10 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="G52" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1763,10 +1943,10 @@
         <v>54</v>
       </c>
       <c r="F54" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="H54" t="s">
-        <v>66</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1780,10 +1960,10 @@
         <v>54</v>
       </c>
       <c r="F55" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="H55" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1800,7 +1980,7 @@
         <v>62</v>
       </c>
       <c r="E56" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -1817,7 +1997,7 @@
         <v>63</v>
       </c>
       <c r="E57" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -1834,7 +2014,7 @@
         <v>64</v>
       </c>
       <c r="E58" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -1848,13 +2028,13 @@
         <v>55</v>
       </c>
       <c r="E59" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="F59" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="H59" t="s">
-        <v>62</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -1871,19 +2051,19 @@
         <v>65</v>
       </c>
       <c r="E60" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="F60" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="G60" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="H60" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="I60" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -1900,19 +2080,19 @@
         <v>66</v>
       </c>
       <c r="E61" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="F61" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="G61" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="H61" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I61" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -1926,22 +2106,22 @@
         <v>56</v>
       </c>
       <c r="D62" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E62" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="F62" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="G62" t="s">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="H62" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="I62" t="s">
-        <v>84</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Bible study condition to grid algorithm and updated example images
</commit_message>
<xml_diff>
--- a/Grids/GetToGrid_Week1.xlsx
+++ b/Grids/GetToGrid_Week1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="89">
   <si>
     <t>Activity</t>
   </si>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Ropes </t>
   </si>
   <si>
-    <t>Lifegaurd</t>
+    <t xml:space="preserve">Lifeguard </t>
   </si>
   <si>
     <t>Speaker Snack</t>
@@ -67,7 +67,7 @@
     <t>Skeet</t>
   </si>
   <si>
-    <t>PPP Lifegaurd</t>
+    <t xml:space="preserve">PPP Lifeguard </t>
   </si>
   <si>
     <t>Blob Spotter</t>
@@ -187,286 +187,100 @@
     <t>11:00-11:45</t>
   </si>
   <si>
-    <t>Nodder Male['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Unicorn Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Opps Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Bow Wow Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Zombie Male['']</t>
-  </si>
-  <si>
-    <t>Nono Male['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Hoops Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>T-Whisk Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Nom Nom Female['']</t>
-  </si>
-  <si>
-    <t>Acro Male['Leadership', 'Male']</t>
-  </si>
-  <si>
-    <t>Zombie Male['Male']</t>
-  </si>
-  <si>
-    <t>Nono Male['']</t>
-  </si>
-  <si>
-    <t>Goobie Female['']</t>
-  </si>
-  <si>
-    <t>Indi Male['']</t>
-  </si>
-  <si>
-    <t>Jaws Male['']</t>
-  </si>
-  <si>
-    <t>Dad Female['Female', 'Leadership']</t>
-  </si>
-  <si>
-    <t>Smiles Female['Female']</t>
-  </si>
-  <si>
-    <t>Laddy Male['Lifegaurd', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Burning Bush Male['Lifegaurd', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Bonez Female['Lifegaurd', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Captain Male['Non-program']</t>
-  </si>
-  <si>
-    <t>Bow Wow Female['Non-program']</t>
-  </si>
-  <si>
-    <t>Tross Male['Lifegaurd', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Pizza Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Ups Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Nom Nom Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Smiles Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Goobie Female['Female']</t>
-  </si>
-  <si>
-    <t>Opps Female['Female']</t>
-  </si>
-  <si>
-    <t>Hoops Female['Female']</t>
-  </si>
-  <si>
-    <t>T-Whisk Female['Female']</t>
-  </si>
-  <si>
-    <t>Captain Male['']</t>
-  </si>
-  <si>
-    <t>Stastro Male['']</t>
-  </si>
-  <si>
-    <t>Chicken Female['']</t>
-  </si>
-  <si>
-    <t>G-Poppy Female['Ropes']</t>
-  </si>
-  <si>
-    <t>Laddy Male['Ropes']</t>
-  </si>
-  <si>
-    <t>Burning Bush Male['Ropes']</t>
-  </si>
-  <si>
-    <t>Bow Wow Female['Ropes']</t>
-  </si>
-  <si>
-    <t>Nodder Male['Ropes']</t>
-  </si>
-  <si>
-    <t>Blister Male['Ropes']</t>
-  </si>
-  <si>
-    <t>GoGo Female['Female']</t>
-  </si>
-  <si>
-    <t>Unicorn Female['Female']</t>
-  </si>
-  <si>
-    <t>Indi Male['Male']</t>
-  </si>
-  <si>
-    <t>GoGo Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Surf Co Male['']</t>
-  </si>
-  <si>
-    <t>Opps Female['']</t>
-  </si>
-  <si>
-    <t>Stastro Male['Male']</t>
-  </si>
-  <si>
-    <t>Sea Female['']</t>
-  </si>
-  <si>
-    <t>Chicken Female['Lifegaurd', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Sea Female['Non-program']</t>
-  </si>
-  <si>
-    <t>Indi Male['Non-program']</t>
-  </si>
-  <si>
-    <t>Laddy Male['Male', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Burning Bush Male['Male', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Sea Female['Lifegaurd', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Chicken Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Indi Male['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Captain Male['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Bonez Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>G-Poppy Female['']</t>
-  </si>
-  <si>
-    <t>T-Whisk Female['']</t>
-  </si>
-  <si>
-    <t>Bow Wow Female['Female']</t>
-  </si>
-  <si>
-    <t>Stastro Male['Ropes']</t>
-  </si>
-  <si>
-    <t>Pizza Female['Ropes']</t>
+    <t>Ups</t>
+  </si>
+  <si>
+    <t>Hoops</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Surf Co</t>
+  </si>
+  <si>
+    <t>Smiles</t>
+  </si>
+  <si>
+    <t>Nom Nom</t>
+  </si>
+  <si>
+    <t>Goobie</t>
+  </si>
+  <si>
+    <t>Nono</t>
+  </si>
+  <si>
+    <t>Acro</t>
+  </si>
+  <si>
+    <t>Indi</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Stastro</t>
+  </si>
+  <si>
+    <t>Dad</t>
+  </si>
+  <si>
+    <t>G-Poppy</t>
+  </si>
+  <si>
+    <t>Bonez</t>
+  </si>
+  <si>
+    <t>Sea</t>
+  </si>
+  <si>
+    <t>Laddy</t>
+  </si>
+  <si>
+    <t>Burning Bush</t>
+  </si>
+  <si>
+    <t>Bow Wow</t>
+  </si>
+  <si>
+    <t>T-Whisk</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>GoGo</t>
+  </si>
+  <si>
+    <t>Hawma</t>
+  </si>
+  <si>
+    <t>Nodder</t>
+  </si>
+  <si>
+    <t>Blister</t>
+  </si>
+  <si>
+    <t>Opps</t>
   </si>
   <si>
     <t>NONE FOUND</t>
   </si>
   <si>
-    <t>Tross Male['Male']</t>
-  </si>
-  <si>
-    <t>Laddy Male['Male']</t>
-  </si>
-  <si>
-    <t>Burning Bush Male['Male']</t>
-  </si>
-  <si>
-    <t>Surf Co Male['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Blister Male['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Tross Male['']</t>
-  </si>
-  <si>
-    <t>Hoops Female['']</t>
-  </si>
-  <si>
-    <t>GoGo Female['']</t>
-  </si>
-  <si>
-    <t>Indi Male['Lifegaurd', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Bow Wow Female['Lifegaurd', 'Non-program']</t>
-  </si>
-  <si>
-    <t>Jaws Male['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Chicken Female['Female']</t>
-  </si>
-  <si>
-    <t>Bonez Female['Female']</t>
-  </si>
-  <si>
-    <t>Pizza Female['Female']</t>
-  </si>
-  <si>
-    <t>Blister Male['']</t>
-  </si>
-  <si>
-    <t>Burning Bush Male['']</t>
-  </si>
-  <si>
-    <t>Sea Female['Female']</t>
-  </si>
-  <si>
-    <t>Nono Male['Male']</t>
-  </si>
-  <si>
-    <t>Laddy Male['Non-program']</t>
-  </si>
-  <si>
-    <t>Burning Bush Male['Non-program']</t>
-  </si>
-  <si>
-    <t>Zombie Male['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Ups Female['Female']</t>
-  </si>
-  <si>
-    <t>Surf Co Male['Male']</t>
-  </si>
-  <si>
-    <t>Pizza Female['']</t>
-  </si>
-  <si>
-    <t>Bow Wow Female['']</t>
-  </si>
-  <si>
-    <t>Bow Wow Female['Ropes', 'Non-program']</t>
-  </si>
-  <si>
-    <t>T-Whisk Female['Ropes', 'Non-program']</t>
-  </si>
-  <si>
-    <t>G-Poppy Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Goobie Female['Lifegaurd']</t>
-  </si>
-  <si>
-    <t>Laddy Male['']</t>
+    <t>Tross</t>
+  </si>
+  <si>
+    <t>Captain</t>
+  </si>
+  <si>
+    <t>Jaws</t>
+  </si>
+  <si>
+    <t>Unicorn</t>
+  </si>
+  <si>
+    <t>Padge</t>
   </si>
 </sst>
 </file>
@@ -867,19 +681,19 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="I2" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -893,19 +707,19 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -919,10 +733,10 @@
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -936,10 +750,10 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I5" t="s">
-        <v>136</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -953,19 +767,19 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -979,19 +793,19 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="H7" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1016,7 +830,7 @@
         <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1030,7 +844,7 @@
         <v>38</v>
       </c>
       <c r="I10" t="s">
-        <v>147</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1044,7 +858,7 @@
         <v>39</v>
       </c>
       <c r="I11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1058,7 +872,7 @@
         <v>39</v>
       </c>
       <c r="I12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1072,7 +886,7 @@
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1086,10 +900,10 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1103,10 +917,10 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1120,10 +934,10 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1137,16 +951,16 @@
         <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="H17" t="s">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="I17" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1160,16 +974,16 @@
         <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>140</v>
+        <v>73</v>
       </c>
       <c r="I18" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1194,7 +1008,7 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1208,7 +1022,7 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1222,7 +1036,7 @@
         <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1236,7 +1050,7 @@
         <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1250,19 +1064,19 @@
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1276,19 +1090,19 @@
         <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="G25" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="H25" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="I25" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1305,19 +1119,19 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="G26" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26" t="s">
         <v>63</v>
-      </c>
-      <c r="H26" t="s">
-        <v>60</v>
-      </c>
-      <c r="I26" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1334,16 +1148,16 @@
         <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F27" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="G27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H27" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="I27" t="s">
         <v>58</v>
@@ -1363,19 +1177,19 @@
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="F28" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I28" t="s">
-        <v>141</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1392,19 +1206,19 @@
         <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="F29" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="G29" t="s">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="H29" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
       <c r="I29" t="s">
-        <v>148</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1418,19 +1232,19 @@
         <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="F30" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="G30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H30" t="s">
-        <v>111</v>
+        <v>57</v>
       </c>
       <c r="I30" t="s">
-        <v>149</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1444,10 +1258,10 @@
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="H31" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1461,10 +1275,10 @@
         <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>116</v>
+        <v>75</v>
       </c>
       <c r="H32" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1478,19 +1292,19 @@
         <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G33" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="H33" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="I33" t="s">
-        <v>137</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1504,19 +1318,19 @@
         <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G34" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="H34" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="I34" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1530,19 +1344,19 @@
         <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="F35" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="G35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H35" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I35" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1556,19 +1370,19 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="F36" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="G36" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="H36" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="I36" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1585,19 +1399,19 @@
         <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F37" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G37" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="H37" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="I37" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1611,13 +1425,13 @@
         <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="G38" t="s">
+        <v>64</v>
+      </c>
+      <c r="I38" t="s">
         <v>61</v>
-      </c>
-      <c r="I38" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1631,13 +1445,13 @@
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G39" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="I39" t="s">
-        <v>128</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1651,13 +1465,13 @@
         <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="G40" t="s">
-        <v>136</v>
+        <v>78</v>
       </c>
       <c r="I40" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1671,19 +1485,19 @@
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F41" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="G41" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H41" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="I41" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1697,19 +1511,19 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F42" t="s">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="G42" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="H42" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="I42" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1723,19 +1537,19 @@
         <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="F43" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="G43" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="H43" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="I43" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1749,19 +1563,19 @@
         <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="F44" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G44" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="H44" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="I44" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1775,19 +1589,19 @@
         <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="F45" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="G45" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="H45" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="I45" t="s">
-        <v>120</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1801,13 +1615,13 @@
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="G46" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="I46" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1821,13 +1635,13 @@
         <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G47" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="I47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1841,10 +1655,10 @@
         <v>52</v>
       </c>
       <c r="F48" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="H48" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1858,16 +1672,16 @@
         <v>47</v>
       </c>
       <c r="E49" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="F49" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H49" t="s">
-        <v>142</v>
+        <v>87</v>
       </c>
       <c r="I49" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1881,10 +1695,10 @@
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>122</v>
+        <v>84</v>
       </c>
       <c r="H50" t="s">
-        <v>143</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1898,10 +1712,10 @@
         <v>48</v>
       </c>
       <c r="F51" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="H51" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1915,10 +1729,10 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="G52" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1943,10 +1757,10 @@
         <v>54</v>
       </c>
       <c r="F54" t="s">
-        <v>124</v>
+        <v>63</v>
       </c>
       <c r="H54" t="s">
-        <v>141</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1960,10 +1774,10 @@
         <v>54</v>
       </c>
       <c r="F55" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="H55" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1980,7 +1794,7 @@
         <v>62</v>
       </c>
       <c r="E56" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -1997,7 +1811,7 @@
         <v>63</v>
       </c>
       <c r="E57" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2011,10 +1825,10 @@
         <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E58" t="s">
-        <v>100</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2028,13 +1842,13 @@
         <v>55</v>
       </c>
       <c r="E59" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="F59" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="H59" t="s">
-        <v>144</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2048,22 +1862,22 @@
         <v>55</v>
       </c>
       <c r="D60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E60" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="F60" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="G60" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="H60" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="I60" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2077,22 +1891,22 @@
         <v>56</v>
       </c>
       <c r="D61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2106,22 +1920,22 @@
         <v>56</v>
       </c>
       <c r="D62" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E62" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F62" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="G62" t="s">
-        <v>138</v>
+        <v>59</v>
       </c>
       <c r="H62" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="I62" t="s">
-        <v>138</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed long term data files
</commit_message>
<xml_diff>
--- a/Grids/GetToGrid_Week1.xlsx
+++ b/Grids/GetToGrid_Week1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="90">
   <si>
     <t>Activity</t>
   </si>
@@ -187,100 +187,103 @@
     <t>11:00-11:45</t>
   </si>
   <si>
+    <t>Goobie</t>
+  </si>
+  <si>
+    <t>Bonez</t>
+  </si>
+  <si>
+    <t>Sea</t>
+  </si>
+  <si>
+    <t>Surf Co</t>
+  </si>
+  <si>
+    <t>Blister</t>
+  </si>
+  <si>
+    <t>Unicorn</t>
+  </si>
+  <si>
+    <t>Smiles</t>
+  </si>
+  <si>
+    <t>Acro</t>
+  </si>
+  <si>
+    <t>Nono</t>
+  </si>
+  <si>
+    <t>Padge</t>
+  </si>
+  <si>
+    <t>Hoops</t>
+  </si>
+  <si>
+    <t>GoGo</t>
+  </si>
+  <si>
+    <t>Gaggles</t>
+  </si>
+  <si>
+    <t>Opps</t>
+  </si>
+  <si>
+    <t>Laddy</t>
+  </si>
+  <si>
+    <t>Jaws</t>
+  </si>
+  <si>
     <t>Ups</t>
   </si>
   <si>
-    <t>Hoops</t>
+    <t>Indi</t>
+  </si>
+  <si>
+    <t>Nom Nom</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>NONE FOUND</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Captain</t>
+  </si>
+  <si>
+    <t>Nodder</t>
+  </si>
+  <si>
+    <t>Stastro</t>
+  </si>
+  <si>
+    <t>Tross</t>
+  </si>
+  <si>
+    <t>Hawma</t>
+  </si>
+  <si>
+    <t>Burning Bush</t>
   </si>
   <si>
     <t>Zombie</t>
   </si>
   <si>
-    <t>Surf Co</t>
-  </si>
-  <si>
-    <t>Smiles</t>
-  </si>
-  <si>
-    <t>Nom Nom</t>
-  </si>
-  <si>
-    <t>Goobie</t>
-  </si>
-  <si>
-    <t>Nono</t>
-  </si>
-  <si>
-    <t>Acro</t>
-  </si>
-  <si>
-    <t>Indi</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>Stastro</t>
-  </si>
-  <si>
     <t>Dad</t>
   </si>
   <si>
+    <t>Bow Wow</t>
+  </si>
+  <si>
     <t>G-Poppy</t>
   </si>
   <si>
-    <t>Bonez</t>
-  </si>
-  <si>
-    <t>Sea</t>
-  </si>
-  <si>
-    <t>Laddy</t>
-  </si>
-  <si>
-    <t>Burning Bush</t>
-  </si>
-  <si>
-    <t>Bow Wow</t>
-  </si>
-  <si>
     <t>T-Whisk</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>GoGo</t>
-  </si>
-  <si>
-    <t>Hawma</t>
-  </si>
-  <si>
-    <t>Nodder</t>
-  </si>
-  <si>
-    <t>Blister</t>
-  </si>
-  <si>
-    <t>Opps</t>
-  </si>
-  <si>
-    <t>NONE FOUND</t>
-  </si>
-  <si>
-    <t>Tross</t>
-  </si>
-  <si>
-    <t>Captain</t>
-  </si>
-  <si>
-    <t>Jaws</t>
-  </si>
-  <si>
-    <t>Unicorn</t>
-  </si>
-  <si>
-    <t>Padge</t>
   </si>
 </sst>
 </file>
@@ -681,19 +684,19 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="H2" t="s">
         <v>75</v>
       </c>
       <c r="I2" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -707,19 +710,19 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
         <v>58</v>
       </c>
-      <c r="H3" t="s">
-        <v>81</v>
-      </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -736,7 +739,7 @@
         <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -753,7 +756,7 @@
         <v>68</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -770,16 +773,16 @@
         <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -796,16 +799,16 @@
         <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="I7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -830,7 +833,7 @@
         <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -844,7 +847,7 @@
         <v>38</v>
       </c>
       <c r="I10" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -858,7 +861,7 @@
         <v>39</v>
       </c>
       <c r="I11" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -872,7 +875,7 @@
         <v>39</v>
       </c>
       <c r="I12" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -886,7 +889,7 @@
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -900,10 +903,10 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -917,10 +920,10 @@
         <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -934,10 +937,10 @@
         <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -951,16 +954,16 @@
         <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I17" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -974,16 +977,16 @@
         <v>42</v>
       </c>
       <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I18" t="s">
         <v>74</v>
-      </c>
-      <c r="F18" t="s">
-        <v>85</v>
-      </c>
-      <c r="H18" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1008,7 +1011,7 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1022,7 +1025,7 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1036,7 +1039,7 @@
         <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1050,7 +1053,7 @@
         <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1064,19 +1067,19 @@
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="G24" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="H24" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="I24" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1090,16 +1093,16 @@
         <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="I25" t="s">
         <v>60</v>
@@ -1119,19 +1122,19 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" t="s">
         <v>57</v>
-      </c>
-      <c r="F26" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" t="s">
-        <v>57</v>
-      </c>
-      <c r="H26" t="s">
-        <v>59</v>
-      </c>
-      <c r="I26" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1148,19 +1151,19 @@
         <v>58</v>
       </c>
       <c r="E27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" t="s">
         <v>59</v>
-      </c>
-      <c r="F27" t="s">
-        <v>59</v>
-      </c>
-      <c r="G27" t="s">
-        <v>60</v>
-      </c>
-      <c r="H27" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1177,19 +1180,19 @@
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F28" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="H28" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="I28" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1206,19 +1209,19 @@
         <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G29" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H29" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1232,19 +1235,19 @@
         <v>48</v>
       </c>
       <c r="E30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" t="s">
+        <v>73</v>
+      </c>
+      <c r="H30" t="s">
         <v>58</v>
       </c>
-      <c r="F30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" t="s">
-        <v>58</v>
-      </c>
-      <c r="H30" t="s">
-        <v>57</v>
-      </c>
       <c r="I30" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1258,10 +1261,10 @@
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="H31" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1275,10 +1278,10 @@
         <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="H32" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1292,19 +1295,19 @@
         <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F33" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="G33" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="H33" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I33" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1318,19 +1321,19 @@
         <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="F34" t="s">
         <v>76</v>
       </c>
       <c r="G34" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H34" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="I34" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1344,19 +1347,19 @@
         <v>50</v>
       </c>
       <c r="E35" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" t="s">
+        <v>77</v>
+      </c>
+      <c r="H35" t="s">
         <v>76</v>
       </c>
-      <c r="F35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" t="s">
-        <v>83</v>
-      </c>
-      <c r="H35" t="s">
-        <v>83</v>
-      </c>
       <c r="I35" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1370,19 +1373,19 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="G36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H36" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="I36" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1399,19 +1402,19 @@
         <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G37" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" t="s">
         <v>66</v>
       </c>
-      <c r="H37" t="s">
-        <v>64</v>
-      </c>
       <c r="I37" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1425,13 +1428,13 @@
         <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I38" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1445,13 +1448,13 @@
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G39" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="I39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1465,13 +1468,13 @@
         <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G40" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="I40" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1485,19 +1488,19 @@
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="F41" t="s">
+        <v>84</v>
+      </c>
+      <c r="G41" t="s">
+        <v>66</v>
+      </c>
+      <c r="H41" t="s">
+        <v>61</v>
+      </c>
+      <c r="I41" t="s">
         <v>81</v>
-      </c>
-      <c r="G41" t="s">
-        <v>88</v>
-      </c>
-      <c r="H41" t="s">
-        <v>79</v>
-      </c>
-      <c r="I41" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1511,19 +1514,19 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="F42" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G42" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H42" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="I42" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1537,19 +1540,19 @@
         <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F43" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="G43" t="s">
         <v>77</v>
       </c>
       <c r="H43" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="I43" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1563,19 +1566,19 @@
         <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="F44" t="s">
+        <v>77</v>
+      </c>
+      <c r="G44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H44" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" t="s">
         <v>88</v>
-      </c>
-      <c r="G44" t="s">
-        <v>70</v>
-      </c>
-      <c r="H44" t="s">
-        <v>80</v>
-      </c>
-      <c r="I44" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1589,19 +1592,19 @@
         <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F45" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G45" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H45" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="I45" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1615,13 +1618,13 @@
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="G46" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I46" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1635,13 +1638,13 @@
         <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G47" t="s">
         <v>62</v>
       </c>
       <c r="I47" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1655,10 +1658,10 @@
         <v>52</v>
       </c>
       <c r="F48" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="H48" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1672,16 +1675,16 @@
         <v>47</v>
       </c>
       <c r="E49" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F49" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H49" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="I49" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1695,10 +1698,10 @@
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H50" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1712,10 +1715,10 @@
         <v>48</v>
       </c>
       <c r="F51" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H51" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1729,10 +1732,10 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G52" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1757,7 +1760,7 @@
         <v>54</v>
       </c>
       <c r="F54" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H54" t="s">
         <v>60</v>
@@ -1774,10 +1777,10 @@
         <v>54</v>
       </c>
       <c r="F55" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H55" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1794,7 +1797,7 @@
         <v>62</v>
       </c>
       <c r="E56" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -1808,10 +1811,10 @@
         <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E57" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -1825,10 +1828,10 @@
         <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E58" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -1842,13 +1845,13 @@
         <v>55</v>
       </c>
       <c r="E59" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="F59" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="H59" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -1862,22 +1865,22 @@
         <v>55</v>
       </c>
       <c r="D60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E60" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="F60" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G60" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="H60" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="I60" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -1891,22 +1894,22 @@
         <v>56</v>
       </c>
       <c r="D61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -1920,22 +1923,22 @@
         <v>56</v>
       </c>
       <c r="D62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E62" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F62" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="G62" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I62" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created randomized index incraments in create grid function
</commit_message>
<xml_diff>
--- a/Grids/GetToGrid_Week1.xlsx
+++ b/Grids/GetToGrid_Week1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="94">
   <si>
     <t>Activity</t>
   </si>
@@ -187,103 +187,115 @@
     <t>11:00-11:45</t>
   </si>
   <si>
+    <t>Hoops</t>
+  </si>
+  <si>
+    <t>Unicorn</t>
+  </si>
+  <si>
+    <t>Bonez</t>
+  </si>
+  <si>
+    <t>Tross</t>
+  </si>
+  <si>
+    <t>Burning Bush</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Nom Nom</t>
+  </si>
+  <si>
+    <t>Sea</t>
+  </si>
+  <si>
+    <t>Bow Wow</t>
+  </si>
+  <si>
+    <t>Swamp Puppy</t>
+  </si>
+  <si>
+    <t>Hawma</t>
+  </si>
+  <si>
+    <t>Hullabaloo</t>
+  </si>
+  <si>
+    <t>Opps</t>
+  </si>
+  <si>
+    <t>Surf Co</t>
+  </si>
+  <si>
+    <t>Indi</t>
+  </si>
+  <si>
+    <t>GoGo</t>
+  </si>
+  <si>
+    <t>Ups</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Smiles</t>
+  </si>
+  <si>
+    <t>NONE FOUND</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Nodder</t>
+  </si>
+  <si>
+    <t>Captain</t>
+  </si>
+  <si>
+    <t>Stastro</t>
+  </si>
+  <si>
+    <t>Laddy</t>
+  </si>
+  <si>
+    <t>Blister</t>
+  </si>
+  <si>
+    <t>Padge</t>
+  </si>
+  <si>
     <t>Goobie</t>
   </si>
   <si>
-    <t>Bonez</t>
-  </si>
-  <si>
-    <t>Sea</t>
-  </si>
-  <si>
-    <t>Surf Co</t>
-  </si>
-  <si>
-    <t>Blister</t>
-  </si>
-  <si>
-    <t>Unicorn</t>
-  </si>
-  <si>
-    <t>Smiles</t>
-  </si>
-  <si>
-    <t>Acro</t>
+    <t>Dad</t>
+  </si>
+  <si>
+    <t>T-Whisk</t>
+  </si>
+  <si>
+    <t>G-Poppy</t>
   </si>
   <si>
     <t>Nono</t>
   </si>
   <si>
-    <t>Padge</t>
-  </si>
-  <si>
-    <t>Hoops</t>
-  </si>
-  <si>
-    <t>GoGo</t>
+    <t>Jaws</t>
+  </si>
+  <si>
+    <t>Socks</t>
   </si>
   <si>
     <t>Gaggles</t>
   </si>
   <si>
-    <t>Opps</t>
-  </si>
-  <si>
-    <t>Laddy</t>
-  </si>
-  <si>
-    <t>Jaws</t>
-  </si>
-  <si>
-    <t>Ups</t>
-  </si>
-  <si>
-    <t>Indi</t>
-  </si>
-  <si>
-    <t>Nom Nom</t>
-  </si>
-  <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>NONE FOUND</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Captain</t>
-  </si>
-  <si>
-    <t>Nodder</t>
-  </si>
-  <si>
-    <t>Stastro</t>
-  </si>
-  <si>
-    <t>Tross</t>
-  </si>
-  <si>
-    <t>Hawma</t>
-  </si>
-  <si>
-    <t>Burning Bush</t>
-  </si>
-  <si>
-    <t>Zombie</t>
-  </si>
-  <si>
-    <t>Dad</t>
-  </si>
-  <si>
-    <t>Bow Wow</t>
-  </si>
-  <si>
-    <t>G-Poppy</t>
-  </si>
-  <si>
-    <t>T-Whisk</t>
+    <t>"2319"</t>
+  </si>
+  <si>
+    <t>Packs</t>
   </si>
 </sst>
 </file>
@@ -684,19 +696,19 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -710,19 +722,19 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" t="s">
         <v>65</v>
       </c>
-      <c r="H3" t="s">
-        <v>58</v>
-      </c>
       <c r="I3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -739,7 +751,7 @@
         <v>67</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -753,10 +765,10 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -770,19 +782,19 @@
         <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -796,19 +808,19 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="G7" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="I7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -833,7 +845,7 @@
         <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -847,7 +859,7 @@
         <v>38</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -861,7 +873,7 @@
         <v>39</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -875,7 +887,7 @@
         <v>39</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -889,7 +901,7 @@
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -903,10 +915,10 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="F14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -923,7 +935,7 @@
         <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -940,7 +952,7 @@
         <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -954,16 +966,16 @@
         <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -977,16 +989,16 @@
         <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H18" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="I18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1025,7 +1037,7 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1039,7 +1051,7 @@
         <v>45</v>
       </c>
       <c r="H22" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1053,7 +1065,7 @@
         <v>45</v>
       </c>
       <c r="H23" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1067,19 +1079,19 @@
         <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="F24" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H24" t="s">
         <v>59</v>
       </c>
       <c r="I24" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1093,19 +1105,19 @@
         <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
         <v>59</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H25" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="I25" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1122,19 +1134,19 @@
         <v>57</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="F26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="H26" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="I26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1151,19 +1163,19 @@
         <v>58</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="G27" t="s">
         <v>57</v>
       </c>
       <c r="H27" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="I27" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1180,19 +1192,19 @@
         <v>59</v>
       </c>
       <c r="E28" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="H28" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="I28" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1209,19 +1221,19 @@
         <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="G29" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="H29" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="I29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1235,16 +1247,16 @@
         <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G30" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H30" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="I30" t="s">
         <v>73</v>
@@ -1261,10 +1273,10 @@
         <v>47</v>
       </c>
       <c r="F31" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="H31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1278,10 +1290,10 @@
         <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="H32" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1295,19 +1307,19 @@
         <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="F33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G33" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="H33" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="I33" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1321,19 +1333,19 @@
         <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G34" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1347,19 +1359,19 @@
         <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G35" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="H35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I35" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1373,19 +1385,19 @@
         <v>48</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G36" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H36" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1402,19 +1414,19 @@
         <v>61</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F37" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="G37" t="s">
+        <v>87</v>
+      </c>
+      <c r="H37" t="s">
         <v>88</v>
       </c>
-      <c r="H37" t="s">
-        <v>66</v>
-      </c>
       <c r="I37" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1428,13 +1440,13 @@
         <v>52</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G38" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="I38" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1448,13 +1460,13 @@
         <v>52</v>
       </c>
       <c r="E39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G39" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="I39" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1468,13 +1480,13 @@
         <v>52</v>
       </c>
       <c r="E40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G40" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I40" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1488,19 +1500,19 @@
         <v>52</v>
       </c>
       <c r="E41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F41" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G41" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="H41" t="s">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="I41" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1514,19 +1526,19 @@
         <v>52</v>
       </c>
       <c r="E42" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" t="s">
         <v>61</v>
       </c>
-      <c r="F42" t="s">
-        <v>65</v>
-      </c>
       <c r="G42" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="H42" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="I42" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1540,19 +1552,19 @@
         <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F43" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="G43" t="s">
         <v>77</v>
       </c>
       <c r="H43" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="I43" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1566,19 +1578,19 @@
         <v>52</v>
       </c>
       <c r="E44" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F44" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="G44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H44" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I44" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1592,19 +1604,19 @@
         <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H45" t="s">
         <v>78</v>
       </c>
       <c r="I45" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1618,13 +1630,13 @@
         <v>52</v>
       </c>
       <c r="E46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I46" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1638,13 +1650,13 @@
         <v>52</v>
       </c>
       <c r="E47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G47" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="I47" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1658,10 +1670,10 @@
         <v>52</v>
       </c>
       <c r="F48" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="H48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -1675,16 +1687,16 @@
         <v>47</v>
       </c>
       <c r="E49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H49" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -1698,10 +1710,10 @@
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H50" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -1715,10 +1727,10 @@
         <v>48</v>
       </c>
       <c r="F51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H51" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -1732,10 +1744,10 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -1760,10 +1772,10 @@
         <v>54</v>
       </c>
       <c r="F54" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="H54" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -1777,10 +1789,10 @@
         <v>54</v>
       </c>
       <c r="F55" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="H55" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -1797,7 +1809,7 @@
         <v>62</v>
       </c>
       <c r="E56" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -1811,10 +1823,10 @@
         <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E57" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -1828,10 +1840,10 @@
         <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="E58" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -1845,13 +1857,13 @@
         <v>55</v>
       </c>
       <c r="E59" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F59" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H59" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -1865,22 +1877,22 @@
         <v>55</v>
       </c>
       <c r="D60" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E60" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F60" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="G60" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H60" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="I60" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -1894,22 +1906,22 @@
         <v>56</v>
       </c>
       <c r="D61" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E61" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F61" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="G61" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="H61" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I61" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -1923,22 +1935,22 @@
         <v>56</v>
       </c>
       <c r="D62" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E62" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="F62" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G62" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I62" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>